<commit_message>
Commit 04/05/2022 actualizacion de documentos y variables
</commit_message>
<xml_diff>
--- a/Data/Input/Plantilla reporte novedades.xlsx
+++ b/Data/Input/Plantilla reporte novedades.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://terpelcol.sharepoint.com/sites/CentrodeAutomatizacinTerpel-Robots/Shared Documents/Robots/Documentación robots/MER - Vive Terpel/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robot.11\Documents\UiPath\Conciliacion EDS\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{C2998E84-E448-4E3F-AD0D-8CD17BE43611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C847B396-5826-4474-B7C8-01843A20B3BA}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-2325" windowWidth="19440" windowHeight="15000" xr2:uid="{D0FEEDE2-8386-41ED-AE46-CD1BC15B7E2D}"/>
+    <workbookView xWindow="-19320" yWindow="-2325" windowWidth="19440" windowHeight="15000"/>
   </bookViews>
   <sheets>
     <sheet name="Diferencias Salesforce - Sateli" sheetId="1" r:id="rId1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>No. Recibo sin PCC</t>
   </si>
@@ -66,122 +65,11 @@
   <si>
     <t>Venta: Fecha de Transacción</t>
   </si>
-  <si>
-    <t>4668828EDS3174</t>
-  </si>
-  <si>
-    <t>EDS BOSTON</t>
-  </si>
-  <si>
-    <t>EDS3174</t>
-  </si>
-  <si>
-    <t>127109</t>
-  </si>
-  <si>
-    <t>254</t>
-  </si>
-  <si>
-    <t>8782039</t>
-  </si>
-  <si>
-    <t>2022-02-01 06:17:00</t>
-  </si>
-  <si>
-    <t>4039593EDS3208</t>
-  </si>
-  <si>
-    <t>EDS PALMIRANA</t>
-  </si>
-  <si>
-    <t>EDS3208</t>
-  </si>
-  <si>
-    <t>0147073132600</t>
-  </si>
-  <si>
-    <t>94330525</t>
-  </si>
-  <si>
-    <t>2022-02-01 06:22:00</t>
-  </si>
-  <si>
-    <t>0135157748300</t>
-  </si>
-  <si>
-    <t>0123633564800</t>
-  </si>
-  <si>
-    <t>No existe en Salesforce</t>
-  </si>
-  <si>
-    <t>3561501EDS0850</t>
-  </si>
-  <si>
-    <t>No existe en Satelite</t>
-  </si>
-  <si>
-    <t>EDS TERPEL ZONA INDUSTRIAL SA</t>
-  </si>
-  <si>
-    <t>EDS0850</t>
-  </si>
-  <si>
-    <t>V-0173313497</t>
-  </si>
-  <si>
-    <t>Bono Fidelización</t>
-  </si>
-  <si>
-    <t>0098446623400</t>
-  </si>
-  <si>
-    <t>2/02/2022 03:53 PM</t>
-  </si>
-  <si>
-    <t>Existe en SalesForce</t>
-  </si>
-  <si>
-    <t>3514956EDS3221</t>
-  </si>
-  <si>
-    <t>EDS TERPEL PASEO DE LA 15</t>
-  </si>
-  <si>
-    <t>EDS3221</t>
-  </si>
-  <si>
-    <t>V-0173343900</t>
-  </si>
-  <si>
-    <t>306403</t>
-  </si>
-  <si>
-    <t>3/02/2022 04:05 AM</t>
-  </si>
-  <si>
-    <t>1346942EDS2084</t>
-  </si>
-  <si>
-    <t>EDS TERPEL SAN JOSE DE QUITO</t>
-  </si>
-  <si>
-    <t>EDS2084</t>
-  </si>
-  <si>
-    <t>V-0173557566</t>
-  </si>
-  <si>
-    <t>0189957648800</t>
-  </si>
-  <si>
-    <t>5/02/2022 06:53 PM</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;\ #,##0"/>
   </numFmts>
@@ -572,32 +460,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47FC71CC-7AE1-4711-9793-37D6FF91E131}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="28.5546875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="24.6640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" style="4" customWidth="1"/>
     <col min="7" max="7" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.88671875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.5546875" style="1"/>
+    <col min="8" max="8" width="20.85546875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -627,239 +515,6 @@
       </c>
       <c r="J1" s="2" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>4668828</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="5">
-        <v>20000</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>4039593</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="5">
-        <v>20000</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
-        <v>4039593</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="5">
-        <v>20000</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>4039593</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="5">
-        <v>20000</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
-        <v>3561501</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" s="5">
-        <v>30000</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <v>3514956</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="5">
-        <v>20000</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>1346942</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I8" s="5">
-        <v>10000</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -868,18 +523,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1086,18 +741,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79A121BA-4B34-4729-897C-C3075E43F231}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB1E8A68-E516-4B49-9529-F0A6A74D3CA4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79A121BA-4B34-4729-897C-C3075E43F231}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>